<commit_message>
chore: Update hour log spreadsheet with latest entries
</commit_message>
<xml_diff>
--- a/hour log.xlsx
+++ b/hour log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10921"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javad/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2758BD5C-A4C8-9C4C-A3AD-CD414C6CA570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523A2536-FD84-2B4D-AB22-7EE73C6BA8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>Subject</t>
   </si>
@@ -187,13 +187,43 @@
     <t>bug fixes</t>
   </si>
   <si>
-    <t>20min</t>
-  </si>
-  <si>
     <t>fix price formatting and recommended cards detail fetch logic</t>
   </si>
   <si>
-    <t>13 hours and 5 minutes</t>
+    <t>fix detail page</t>
+  </si>
+  <si>
+    <t>5 min</t>
+  </si>
+  <si>
+    <t>fix: increase media query breakpoint for mobile responsiveness on house details page</t>
+  </si>
+  <si>
+    <t>fix console.log</t>
+  </si>
+  <si>
+    <t>fix: remove all console.logs</t>
+  </si>
+  <si>
+    <t>3 min</t>
+  </si>
+  <si>
+    <t>refactor components/views</t>
+  </si>
+  <si>
+    <t>- Introduced FormRow and FormField components for better form structure and reusability. - Implemented ImageUpload component for handling image uploads with preview functionality. - Created SelectField component for dropdown selections. - Replaced existing form elements in CreateHouseView with new components for consistency and maintainability. - Added NoResults component to standardize no results display across views. - Refactored FavoritesView and HousesView to utilize new components for search and sorting functionality.</t>
+  </si>
+  <si>
+    <t>fix form errors</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <t>enhance form error handeling by adding red border and red place holder</t>
+  </si>
+  <si>
+    <t>14 hours and 58 minutes</t>
   </si>
 </sst>
 </file>
@@ -301,7 +331,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -471,6 +501,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -489,7 +530,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -552,6 +593,12 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1813,7 +1860,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2066,46 +2113,78 @@
         <v>43</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C16" s="18">
         <v>45917</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
+      <c r="A17" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="18">
+        <v>45926</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>47</v>
+      </c>
       <c r="E17" s="15"/>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
+      <c r="A18" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="18">
+        <v>45926</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>49</v>
+      </c>
       <c r="E18" s="15"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
+    <row r="19" spans="1:6" ht="213" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="22">
+        <v>45926</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>52</v>
+      </c>
       <c r="E19" s="15"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="19"/>
+      <c r="A20" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="22">
+        <v>45926</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>55</v>
+      </c>
       <c r="E20" s="15"/>
       <c r="F20" s="4"/>
     </row>
@@ -2186,7 +2265,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>